<commit_message>
fix[DE]: Adjust tests for CandidateInstance
</commit_message>
<xml_diff>
--- a/DataSetExplorerTests/DataFactories/TestData/BurningKnight2.xlsx
+++ b/DataSetExplorerTests/DataFactories/TestData/BurningKnight2.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lubur\Documents\Fakultet\!PROJEKTI\Clean CaDET\PLATFORM\platform-repository-compiler\DataSetExplorerTests\DataFactories\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ccadet\platform\DataSetExplorerTests\DataFactories\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AEB4A4-FACA-4FF5-B273-4D1E0DAC29DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA8C601-7AB9-42E5-BABB-0D0DA49539BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Long Method Smell" sheetId="1" r:id="rId1"/>
-    <sheet name="Large Class Smell" sheetId="2" r:id="rId2"/>
+    <sheet name="Long Method" sheetId="1" r:id="rId1"/>
+    <sheet name="Large Class" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1975,24 +1975,24 @@
   </sheetPr>
   <dimension ref="A1:M308"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J203" sqref="J203"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3046875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.109375" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" style="40" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="61.07421875" customWidth="1"/>
+    <col min="2" max="2" width="10.765625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="10.765625" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="11.69140625" customWidth="1"/>
+    <col min="10" max="10" width="11.69140625" customWidth="1"/>
+    <col min="12" max="12" width="11.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>457</v>
       </c>
@@ -2015,7 +2015,7 @@
       <c r="L1" s="47"/>
       <c r="M1" s="47"/>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>460</v>
       </c>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="M2" s="50"/>
     </row>
-    <row r="3" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
@@ -2122,7 +2122,7 @@
       </c>
       <c r="M4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
@@ -2155,7 +2155,7 @@
       </c>
       <c r="M5" s="10"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="M6" s="12"/>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>19</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>21</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>22</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>23</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>24</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>27</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>28</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>31</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>34</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>36</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>37</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>38</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>39</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>40</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>41</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>42</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>43</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>44</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>45</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>46</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>47</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>48</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>49</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>50</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>51</v>
       </c>
@@ -3129,7 +3129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>52</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>53</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>54</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>55</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>56</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>57</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>58</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>59</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>60</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>61</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>62</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>63</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>64</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>65</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>66</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>67</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>68</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>69</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>70</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>71</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>72</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>73</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>74</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>75</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>76</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>77</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>78</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>79</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A73" s="32" t="s">
         <v>80</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>81</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>82</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>83</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>84</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>85</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>86</v>
       </c>
@@ -4002,7 +4002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>87</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>88</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>89</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>90</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>91</v>
       </c>
@@ -4130,7 +4130,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>92</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>93</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A87" s="32" t="s">
         <v>94</v>
       </c>
@@ -4201,7 +4201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
         <v>95</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
         <v>96</v>
       </c>
@@ -4249,7 +4249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
         <v>97</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
         <v>98</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
         <v>99</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A93" s="32" t="s">
         <v>100</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
         <v>101</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
         <v>102</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
         <v>103</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="97" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A97" s="32" t="s">
         <v>104</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
         <v>105</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
         <v>106</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>107</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>108</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>109</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>110</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
         <v>111</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
         <v>112</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>113</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>114</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>115</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>116</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
         <v>117</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
         <v>118</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
         <v>119</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>120</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
         <v>121</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
         <v>122</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
         <v>123</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A117" s="7" t="s">
         <v>124</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>125</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>126</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>127</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>128</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A122" s="32" t="s">
         <v>129</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>130</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>131</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>132</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>133</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
         <v>134</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
         <v>135</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
         <v>136</v>
       </c>
@@ -5236,7 +5236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
         <v>137</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>138</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
         <v>139</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>140</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>141</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>142</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>143</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>144</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A138" s="7" t="s">
         <v>145</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>146</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>147</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>148</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>149</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>150</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>151</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
         <v>152</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
         <v>153</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
         <v>154</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
         <v>155</v>
       </c>
@@ -5720,7 +5720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
         <v>156</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
         <v>157</v>
       </c>
@@ -5772,7 +5772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
         <v>158</v>
       </c>
@@ -5796,7 +5796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A152" s="7" t="s">
         <v>159</v>
       </c>
@@ -5823,7 +5823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
         <v>160</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
         <v>161</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
         <v>162</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
         <v>163</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
         <v>164</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>165</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
         <v>166</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
         <v>167</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
         <v>168</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A162" s="7" t="s">
         <v>169</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
         <v>170</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A164" s="7" t="s">
         <v>171</v>
       </c>
@@ -6123,7 +6123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
         <v>172</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A166" s="7" t="s">
         <v>173</v>
       </c>
@@ -6171,7 +6171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>174</v>
       </c>
@@ -6195,7 +6195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A168" s="32" t="s">
         <v>175</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>176</v>
       </c>
@@ -6242,7 +6242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>177</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>178</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
         <v>179</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
         <v>180</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
         <v>181</v>
       </c>
@@ -6377,7 +6377,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
         <v>182</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
         <v>183</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
         <v>184</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>185</v>
       </c>
@@ -6476,7 +6476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>186</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="180" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
         <v>187</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
         <v>188</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
         <v>189</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A183" s="7" t="s">
         <v>190</v>
       </c>
@@ -6599,7 +6599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
         <v>191</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
         <v>192</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A186" s="7" t="s">
         <v>193</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
         <v>194</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
         <v>195</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
         <v>196</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
         <v>197</v>
       </c>
@@ -6776,7 +6776,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
         <v>198</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="192" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
         <v>199</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>200</v>
       </c>
@@ -6851,7 +6851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
         <v>201</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>202</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>203</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="197" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>204</v>
       </c>
@@ -6956,7 +6956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>205</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="199" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A199" s="32" t="s">
         <v>206</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="200" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>207</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="201" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
         <v>208</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
         <v>209</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
         <v>210</v>
       </c>
@@ -7113,7 +7113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="204" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A204" s="7" t="s">
         <v>211</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="205" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
         <v>212</v>
       </c>
@@ -7161,7 +7161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="206" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
         <v>213</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A207" s="7" t="s">
         <v>214</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A208" s="7" t="s">
         <v>215</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="209" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
         <v>216</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="210" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A210" s="7" t="s">
         <v>217</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A211" s="7" t="s">
         <v>218</v>
       </c>
@@ -7311,7 +7311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="212" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
         <v>219</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="213" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>220</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
         <v>221</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
         <v>222</v>
       </c>
@@ -7407,7 +7407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
         <v>223</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="217" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A217" s="7" t="s">
         <v>224</v>
       </c>
@@ -7461,7 +7461,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="218" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A218" s="7" t="s">
         <v>225</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="219" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A219" s="7" t="s">
         <v>226</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
         <v>227</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="221" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
         <v>228</v>
       </c>
@@ -7560,7 +7560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="222" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A222" s="7" t="s">
         <v>229</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="223" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A223" s="7" t="s">
         <v>230</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="224" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A224" s="7" t="s">
         <v>231</v>
       </c>
@@ -7632,7 +7632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="225" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A225" s="7" t="s">
         <v>232</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A226" s="7" t="s">
         <v>233</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
         <v>234</v>
       </c>
@@ -7704,7 +7704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A228" s="7" t="s">
         <v>235</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="229" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A229" s="7" t="s">
         <v>236</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A230" s="7" t="s">
         <v>237</v>
       </c>
@@ -7779,7 +7779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="231" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A231" s="7" t="s">
         <v>238</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="232" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A232" s="7" t="s">
         <v>239</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A233" s="7" t="s">
         <v>240</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="234" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A234" s="7" t="s">
         <v>241</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A235" s="7" t="s">
         <v>242</v>
       </c>
@@ -7914,7 +7914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="236" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A236" s="7" t="s">
         <v>243</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="237" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A237" s="7" t="s">
         <v>244</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A238" s="7" t="s">
         <v>245</v>
       </c>
@@ -7997,7 +7997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="239" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A239" s="7" t="s">
         <v>246</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="240" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A240" s="7" t="s">
         <v>247</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A241" s="7" t="s">
         <v>248</v>
       </c>
@@ -8078,7 +8078,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="242" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A242" s="32" t="s">
         <v>249</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A243" s="7" t="s">
         <v>250</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="244" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A244" s="7" t="s">
         <v>251</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="245" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A245" s="7" t="s">
         <v>252</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A246" s="6" t="s">
         <v>253</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A247" s="7" t="s">
         <v>254</v>
       </c>
@@ -8224,7 +8224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A248" s="7" t="s">
         <v>255</v>
       </c>
@@ -8248,7 +8248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="249" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A249" s="7" t="s">
         <v>256</v>
       </c>
@@ -8272,7 +8272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A250" s="6" t="s">
         <v>257</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A251" s="7" t="s">
         <v>258</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="252" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A252" s="7" t="s">
         <v>259</v>
       </c>
@@ -8350,7 +8350,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A253" s="6" t="s">
         <v>260</v>
       </c>
@@ -8374,7 +8374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="254" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A254" s="7" t="s">
         <v>261</v>
       </c>
@@ -8398,7 +8398,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="255" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A255" s="7" t="s">
         <v>262</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="256" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A256" s="7" t="s">
         <v>263</v>
       </c>
@@ -8452,7 +8452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A257" s="7" t="s">
         <v>264</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="258" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A258" s="7" t="s">
         <v>265</v>
       </c>
@@ -8500,7 +8500,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A259" s="32" t="s">
         <v>266</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="260" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A260" s="7" t="s">
         <v>267</v>
       </c>
@@ -8550,7 +8550,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="261" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A261" s="7" t="s">
         <v>268</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="262" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A262" s="7" t="s">
         <v>269</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A263" s="7" t="s">
         <v>270</v>
       </c>
@@ -8622,7 +8622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A264" s="7" t="s">
         <v>271</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="265" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A265" s="7" t="s">
         <v>272</v>
       </c>
@@ -8673,7 +8673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A266" s="7" t="s">
         <v>273</v>
       </c>
@@ -8697,7 +8697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="267" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A267" s="32" t="s">
         <v>274</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A268" s="7" t="s">
         <v>275</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="269" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A269" s="7" t="s">
         <v>276</v>
       </c>
@@ -8777,7 +8777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="270" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A270" s="7" t="s">
         <v>277</v>
       </c>
@@ -8804,7 +8804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A271" s="6" t="s">
         <v>278</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="272" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A272" s="7" t="s">
         <v>279</v>
       </c>
@@ -8855,7 +8855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="273" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A273" s="7" t="s">
         <v>280</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="274" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A274" s="7" t="s">
         <v>281</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="275" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A275" s="7" t="s">
         <v>282</v>
       </c>
@@ -8936,7 +8936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="276" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A276" s="7" t="s">
         <v>283</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="277" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A277" s="7" t="s">
         <v>284</v>
       </c>
@@ -8990,7 +8990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="278" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A278" s="7" t="s">
         <v>285</v>
       </c>
@@ -9017,7 +9017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A279" s="7" t="s">
         <v>286</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="280" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A280" s="7" t="s">
         <v>287</v>
       </c>
@@ -9068,7 +9068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A281" s="7" t="s">
         <v>288</v>
       </c>
@@ -9095,7 +9095,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="282" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A282" s="7" t="s">
         <v>289</v>
       </c>
@@ -9122,7 +9122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="283" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A283" s="7" t="s">
         <v>290</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A284" s="7" t="s">
         <v>291</v>
       </c>
@@ -9173,7 +9173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="285" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A285" s="7" t="s">
         <v>292</v>
       </c>
@@ -9200,7 +9200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A286" s="7" t="s">
         <v>293</v>
       </c>
@@ -9224,7 +9224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="287" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A287" s="7" t="s">
         <v>294</v>
       </c>
@@ -9248,7 +9248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="288" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A288" s="7" t="s">
         <v>295</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="289" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A289" s="7" t="s">
         <v>296</v>
       </c>
@@ -9296,7 +9296,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="290" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A290" s="7" t="s">
         <v>297</v>
       </c>
@@ -9320,7 +9320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="291" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A291" s="7" t="s">
         <v>298</v>
       </c>
@@ -9344,7 +9344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="292" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A292" s="7" t="s">
         <v>299</v>
       </c>
@@ -9368,7 +9368,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="293" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A293" s="7" t="s">
         <v>300</v>
       </c>
@@ -9392,7 +9392,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A294" s="7" t="s">
         <v>301</v>
       </c>
@@ -9416,7 +9416,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="295" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A295" s="7" t="s">
         <v>302</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="296" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A296" s="7" t="s">
         <v>303</v>
       </c>
@@ -9464,7 +9464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="297" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A297" s="7" t="s">
         <v>304</v>
       </c>
@@ -9488,7 +9488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A298" s="7" t="s">
         <v>305</v>
       </c>
@@ -9512,7 +9512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="299" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A299" s="7" t="s">
         <v>306</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="300" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A300" s="7" t="s">
         <v>307</v>
       </c>
@@ -9560,7 +9560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="301" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A301" s="7" t="s">
         <v>308</v>
       </c>
@@ -9587,7 +9587,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="302" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A302" s="32" t="s">
         <v>309</v>
       </c>
@@ -9610,7 +9610,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A303" s="7" t="s">
         <v>310</v>
       </c>
@@ -9634,7 +9634,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A304" s="7" t="s">
         <v>311</v>
       </c>
@@ -9658,7 +9658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="305" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A305" s="7" t="s">
         <v>312</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A306" s="7" t="s">
         <v>313</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A307" s="7" t="s">
         <v>314</v>
       </c>
@@ -9730,7 +9730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="308" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A308" s="7" t="s">
         <v>315</v>
       </c>
@@ -9826,23 +9826,23 @@
   </sheetPr>
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.3046875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.21875" customWidth="1"/>
-    <col min="2" max="2" width="37.21875" style="40" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.23046875" customWidth="1"/>
+    <col min="2" max="2" width="37.23046875" style="40" customWidth="1"/>
+    <col min="3" max="3" width="14.3046875" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" customWidth="1"/>
+    <col min="6" max="6" width="11.69140625" customWidth="1"/>
+    <col min="8" max="8" width="11.69140625" customWidth="1"/>
+    <col min="10" max="10" width="11.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>457</v>
       </c>
@@ -9863,7 +9863,7 @@
       <c r="J1" s="47"/>
       <c r="K1" s="47"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="43" t="s">
         <v>460</v>
       </c>
@@ -9890,7 +9890,7 @@
       </c>
       <c r="K2" s="50"/>
     </row>
-    <row r="3" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>319</v>
       </c>
@@ -9946,7 +9946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>320</v>
       </c>
@@ -9976,7 +9976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>321</v>
       </c>
@@ -9997,7 +9997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>322</v>
       </c>
@@ -10018,7 +10018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>323</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>324</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="34" t="s">
         <v>325</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
         <v>326</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>327</v>
       </c>
@@ -10123,7 +10123,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>328</v>
       </c>
@@ -10151,7 +10151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>329</v>
       </c>
@@ -10179,7 +10179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>330</v>
       </c>
@@ -10200,7 +10200,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>331</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>332</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>333</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>334</v>
       </c>
@@ -10289,7 +10289,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="32" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>335</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>336</v>
       </c>
@@ -10330,7 +10330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>337</v>
       </c>
@@ -10351,7 +10351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>338</v>
       </c>
@@ -10372,7 +10372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>339</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>340</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>341</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>342</v>
       </c>
@@ -10456,7 +10456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>343</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>344</v>
       </c>
@@ -10505,7 +10505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>345</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>346</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>347</v>
       </c>
@@ -10571,7 +10571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>348</v>
       </c>
@@ -10595,7 +10595,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>349</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>350</v>
       </c>
@@ -10637,7 +10637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A36" s="32" t="s">
         <v>351</v>
       </c>
@@ -10657,7 +10657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="32" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A37" s="32" t="s">
         <v>352</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>353</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>354</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>355</v>
       </c>
@@ -10746,7 +10746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>356</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>357</v>
       </c>
@@ -10789,7 +10789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>358</v>
       </c>
@@ -10814,7 +10814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>359</v>
       </c>
@@ -10835,7 +10835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>360</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>361</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>362</v>
       </c>
@@ -10898,7 +10898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>363</v>
       </c>
@@ -10919,7 +10919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>364</v>
       </c>
@@ -10940,7 +10940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>365</v>
       </c>
@@ -10961,7 +10961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>366</v>
       </c>
@@ -10982,7 +10982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>367</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>368</v>
       </c>
@@ -11024,7 +11024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>369</v>
       </c>
@@ -11045,7 +11045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>370</v>
       </c>
@@ -11066,7 +11066,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>371</v>
       </c>
@@ -11090,7 +11090,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>372</v>
       </c>
@@ -11111,7 +11111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>373</v>
       </c>
@@ -11135,7 +11135,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>374</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>375</v>
       </c>
@@ -11177,7 +11177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>376</v>
       </c>
@@ -11198,7 +11198,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>377</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>378</v>
       </c>
@@ -11240,7 +11240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>379</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>380</v>
       </c>
@@ -11288,7 +11288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>381</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>382</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>383</v>
       </c>
@@ -11354,7 +11354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>384</v>
       </c>
@@ -11375,7 +11375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>385</v>
       </c>
@@ -11396,7 +11396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>386</v>
       </c>
@@ -11417,7 +11417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>387</v>
       </c>
@@ -11444,7 +11444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>388</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>389</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>390</v>
       </c>
@@ -11510,7 +11510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>391</v>
       </c>
@@ -11531,7 +11531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>392</v>
       </c>
@@ -11552,7 +11552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>393</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>394</v>
       </c>
@@ -11600,7 +11600,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>395</v>
       </c>
@@ -11624,7 +11624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>396</v>
       </c>
@@ -11648,7 +11648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="12.45" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>397</v>
       </c>

</xml_diff>